<commit_message>
Fix today's date and duplicate .xlsx
</commit_message>
<xml_diff>
--- a/AccountsDone.xlsx
+++ b/AccountsDone.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:G66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -501,7 +501,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>(("'NoneType' object has no attribute 'is_displayed'",), 'Attribute not found.')</t>
+          <t>No BNP Invoice</t>
         </is>
       </c>
     </row>
@@ -534,7 +534,11 @@
           <t>TRINA SOLAR-HIH LOGISTICS,INC.FONTANA/POOLER</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -565,7 +569,11 @@
           <t>ALL MARKET INC / VITA COCO</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr"/>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -596,7 +604,11 @@
           <t>ALL MARKET INC / VITA COCO</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -627,7 +639,11 @@
           <t>ALL MARKET INC / VITA COCO</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr"/>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -658,51 +674,57 @@
           <t>ALL MARKET INC / VITA COCO</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr"/>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>CIRCUITCITYCORPORATIONINC</t>
+          <t>ZOOMGETLLC</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Kent</t>
+          <t>Valley View</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Bimonthly</t>
+          <t>Weekly</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>CIRCUIT CITY CORPORATION INC</t>
+          <t>ZOOMGET, LLC</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>CIRCUIT CITY CORPORATION INC</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr"/>
+          <t>ZOOMGET, LLC</t>
+        </is>
+      </c>
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Aterian</t>
+          <t>CIRCUITCITYCORPORATIONINC</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Savannah</t>
+          <t>Kent</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -712,28 +734,32 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>ATERIAN GROUP, INC.</t>
+          <t>CIRCUIT CITY CORPORATION INC</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>ATERIAN GROUP, INC.</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr"/>
+          <t>CIRCUIT CITY CORPORATION INC</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>July&amp;CoPTYLTD</t>
+          <t>Aterian</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Grand Prairie</t>
+          <t>Savannah</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -743,59 +769,65 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>JULY &amp; CO PTY LTD</t>
+          <t>ATERIAN GROUP, INC.</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>JULY &amp; CO PTY LTD</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr"/>
+          <t>ATERIAN GROUP, INC.</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>LeeKumKee</t>
+          <t>DeerStags</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Valley View</t>
+          <t>Kent</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Bimonthly</t>
+          <t>Weekly</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>LEE KUM KEE (U.S.A.) INC.</t>
+          <t>DEER STAGS</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>LEE KUM KEE (U.S.A.) INC.</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr"/>
+          <t>DEER STAGS</t>
+        </is>
+      </c>
+      <c r="G11" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>LunaWellnessLLC</t>
+          <t>July&amp;CoPTYLTD</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>New Jersey</t>
+          <t>Grand Prairie</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -805,28 +837,32 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Luna Wellness LLC</t>
+          <t>JULY &amp; CO PTY LTD</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Luna Wellness LLC</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr"/>
+          <t>JULY &amp; CO PTY LTD</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>OuterInc</t>
+          <t>LeeKumKee</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Willow</t>
+          <t>Valley View</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -836,28 +872,32 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>OUTER, INC</t>
+          <t>LEE KUM KEE (U.S.A.) INC.</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>OUTER, INC</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr"/>
+          <t>LEE KUM KEE (U.S.A.) INC.</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Planahead</t>
+          <t>LunaWellnessLLC</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Fontana</t>
+          <t>New Jersey</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -867,28 +907,32 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>PLANAHEAD</t>
+          <t>Luna Wellness LLC</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>PLANAHEAD,LLC.</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr"/>
+          <t>Luna Wellness LLC</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>SGCompany</t>
+          <t>OuterInc</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Valley View</t>
+          <t>Willow</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -898,28 +942,32 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>THE SG COMPANIES</t>
+          <t>OUTER, INC</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>THE SG COMPANIES</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr"/>
+          <t>OUTER, INC</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>BexcoEnterprises</t>
+          <t>Planahead</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>New Jersey</t>
+          <t>Fontana</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -929,28 +977,32 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>BEXCO ENTERPRISES, INC</t>
+          <t>PLANAHEAD</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>MILLION DOLLAR BABY</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr"/>
+          <t>PLANAHEAD,LLC.</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>SimpleModern</t>
+          <t>SGCompany</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Fontana</t>
+          <t>Valley View</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -960,90 +1012,98 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>SIMPLE MODERN</t>
+          <t>THE SG COMPANIES</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>SIMPLE MODERN</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr"/>
+          <t>THE SG COMPANIES</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>SunriseGlobalMarketing</t>
+          <t>SGCompany</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Tacoma</t>
+          <t>Valley View</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Bimonthly</t>
+          <t>Weekly</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>SUNRISE GLOBAL MARKETING, LLC</t>
+          <t>THE SG COMPANIES</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>SUNRISE GLOBAL MARKETING, LLC</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr"/>
+          <t>THE SG COMPANIES</t>
+        </is>
+      </c>
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>SunriseGlobalMarketing</t>
+          <t>ZOOMGETLLC</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Charleston</t>
+          <t>Murphy</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Bimonthly</t>
+          <t>Weekly</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>SUNRISE GLOBAL MARKETING, LLC</t>
+          <t>ZOOMGET, LLC</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>SUNRISE GLOBAL MARKETING, LLC</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr"/>
+          <t>ZOOMGET, LLC</t>
+        </is>
+      </c>
+      <c r="G19" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>SansWine&amp;Spirits</t>
+          <t>BexcoEnterprises</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Valley View</t>
+          <t>New Jersey</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1053,28 +1113,32 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>SANS WINE &amp; SPIRITS</t>
+          <t>BEXCO ENTERPRISES, INC</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Sans Wine &amp; Spirits</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr"/>
+          <t>MILLION DOLLAR BABY</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>ToughbuiltIndustries</t>
+          <t>SimpleModern</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Morgan Lakes</t>
+          <t>Fontana</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1084,28 +1148,32 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>TOUGHBUILT INDUSTRIES, INC.</t>
+          <t>SIMPLE MODERN</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>TOUGHBUILT INDUSTRIES, INC.</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr"/>
+          <t>SIMPLE MODERN</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>EuromarketDesignsInc</t>
+          <t>SunriseGlobalMarketing</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Valley View</t>
+          <t>Tacoma</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1115,28 +1183,32 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Euromarket Designs, Inc.</t>
+          <t>SUNRISE GLOBAL MARKETING, LLC</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Euromarket Designs, Inc.</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr"/>
+          <t>SUNRISE GLOBAL MARKETING, LLC</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>InternationalTextile&amp;ApparelInc</t>
+          <t>SunriseGlobalMarketing</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Savannah</t>
+          <t>Charleston</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1146,28 +1218,32 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>INTERNATIONAL TEXTILE &amp; APPAREL, INC</t>
+          <t>SUNRISE GLOBAL MARKETING, LLC</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>INTERNATIONAL TEXTILE &amp; APPAREL</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr"/>
+          <t>SUNRISE GLOBAL MARKETING, LLC</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>CastleryUSA</t>
+          <t>SansWine&amp;Spirits</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Kent</t>
+          <t>Valley View</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1177,28 +1253,32 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>CASTLERY USA</t>
+          <t>SANS WINE &amp; SPIRITS</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>CASTLERY USA</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr"/>
+          <t>Sans Wine &amp; Spirits</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>TheFiftyFiftyGroup</t>
+          <t>ToughbuiltIndustries</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Valley View</t>
+          <t>Morgan Lakes</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1208,28 +1288,32 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>THE FIFTY/FIFTY GROUP, INC DBA LOLA PRODUCTS</t>
+          <t>TOUGHBUILT INDUSTRIES, INC.</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>THE FIFTY/FIFTY GROUP, INC DBA LOLA PRODUCTS</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr"/>
+          <t>TOUGHBUILT INDUSTRIES, INC.</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>JSONICSERVICES</t>
+          <t>EuromarketDesignsInc</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Redbluff</t>
+          <t>Valley View</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1239,28 +1323,32 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>JSONIC SERVICES INC</t>
+          <t>Euromarket Designs, Inc.</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>JSONIC SERVICES INC</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr"/>
+          <t>Euromarket Designs, Inc.</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>CoolerMaster</t>
+          <t>InternationalTextile&amp;ApparelInc</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Valley View</t>
+          <t>Savannah</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1270,28 +1358,32 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>COOLER MASTER</t>
+          <t>INTERNATIONAL TEXTILE &amp; APPAREL, INC</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>COOLER MASTER</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr"/>
+          <t>INTERNATIONAL TEXTILE &amp; APPAREL</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>TCUTradingLTD</t>
+          <t>CastleryUSA</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Greenwood</t>
+          <t>Kent</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1301,28 +1393,32 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>TCU TRADING LTD</t>
+          <t>CASTLERY USA</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>TCU TRADING LTD</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr"/>
+          <t>CASTLERY USA</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>GalanzAmericasLimitedCompany</t>
+          <t>TheFiftyFiftyGroup</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Innovation</t>
+          <t>Valley View</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1332,59 +1428,65 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>GALANZ AMERICAS LIMITED COMPANY</t>
+          <t>THE FIFTY/FIFTY GROUP, INC DBA LOLA PRODUCTS</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>GALANZ AMERICAS LIMITED COMPANY</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr"/>
+          <t>THE FIFTY/FIFTY GROUP, INC DBA LOLA PRODUCTS</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>SCHC-Wilsonart</t>
+          <t>TytusGrillsLLC</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>New Jersey</t>
+          <t>Valley View</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Bimonthly</t>
+          <t>Weekly</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>SCHC - Wilsonart</t>
+          <t>TYTUS GRILLS, LLC</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>SCHC - Wilsonart</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr"/>
+          <t>THE FIFTY/FIFTY GROUP, INC DBA LOLA PRODUCTS</t>
+        </is>
+      </c>
+      <c r="G30" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>AcmeFoodSales</t>
+          <t>JSONICSERVICES</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Morgan Lakes</t>
+          <t>Redbluff</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1394,28 +1496,32 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>ACME FOOD SALES INC</t>
+          <t>JSONIC SERVICES INC</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>ACME FOOD SALES INC</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr"/>
+          <t>JSONIC SERVICES INC</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>AterianGroupInc</t>
+          <t>CoolerMaster</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Greenwood</t>
+          <t>Valley View</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1425,28 +1531,32 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>ATERIAN GROUP, INC.</t>
+          <t>COOLER MASTER</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>ATERIAN GROUP, INC.</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr"/>
+          <t>COOLER MASTER</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>BASportsNutrition</t>
+          <t>TCUTradingLTD</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Kansas</t>
+          <t>Greenwood</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1456,28 +1566,32 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>BA SPORTS NUTRITION LLC</t>
+          <t>TCU TRADING LTD</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>BA SPORTS NUTRITION LLC</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr"/>
+          <t>TCU TRADING LTD</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>BanyanInternational</t>
+          <t>GalanzAmericasLimitedCompany</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Indiana</t>
+          <t>Innovation</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1487,28 +1601,32 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>BANYAN INTERNATIONAL</t>
+          <t>GALANZ AMERICAS LIMITED COMPANY</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>BANYAN INTERNATIONAL</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr"/>
+          <t>GALANZ AMERICAS LIMITED COMPANY</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>EPI</t>
+          <t>SCHC-Wilsonart</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Valley View</t>
+          <t>New Jersey</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1518,90 +1636,98 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>ENVISION PERIPHERALS INC.(EPI Non-Bonded)</t>
+          <t>SCHC - Wilsonart</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Envision Peripherals, Inc</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr"/>
+          <t>SCHC - Wilsonart</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>IntradecoIvory</t>
+          <t>TytusGrillsLLC</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>New Jersey</t>
+          <t>Morgan Lakes</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Bimonthly</t>
+          <t>Weekly</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>INTRADECO-IVORY</t>
+          <t>TYTUS GRILLS, LLC</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>INTRADECO-IVORY</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr"/>
+          <t>TYTUS GRILLS, LLC</t>
+        </is>
+      </c>
+      <c r="G36" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>IntradecoKnothe</t>
+          <t>DeltaElectronics</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Morgan Lakes</t>
+          <t>Valley View</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Bimonthly</t>
+          <t>Weekly</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>INTRADECO-KNOTHE</t>
+          <t>DELTA ELECTRONICS</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>INTRADECO-KNOTHE</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr"/>
+          <t>DELTA ELECTRONICS (AMERICAS)LTD-NEW</t>
+        </is>
+      </c>
+      <c r="G37" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>King'sHawaiian</t>
+          <t>AcmeFoodSales</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Valley View</t>
+          <t>Morgan Lakes</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1611,28 +1737,32 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>KING'S HAWAIIAN</t>
+          <t>ACME FOOD SALES INC</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>KING'S HAWAIIAN</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr"/>
+          <t>ACME FOOD SALES INC</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Pepsico</t>
+          <t>AterianGroupInc</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Tacoma</t>
+          <t>Greenwood</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1642,28 +1772,32 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>PEPSICO</t>
+          <t>ATERIAN GROUP, INC.</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>PEPSICO</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr"/>
+          <t>ATERIAN GROUP, INC.</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>LunaWellnessLLC</t>
+          <t>BASportsNutrition</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Valley View</t>
+          <t>Kansas</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1673,28 +1807,32 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Luna Wellness LLC</t>
+          <t>BA SPORTS NUTRITION LLC</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Luna Wellness LLC</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr"/>
+          <t>BA SPORTS NUTRITION LLC</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>SharkNinja</t>
+          <t>BanyanInternational</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Fontana</t>
+          <t>Indiana</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1704,28 +1842,32 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Shark Ninja</t>
+          <t>BANYAN INTERNATIONAL</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>SharkNinja Sales Company</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr"/>
+          <t>BANYAN INTERNATIONAL</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>OtisMcallister</t>
+          <t>EPI</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Valley View</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1735,28 +1877,32 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>OTIS MCALLISTER, INC</t>
+          <t>ENVISION PERIPHERALS INC.(EPI Non-Bonded)</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>OTIS MCALLISTER, INC</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr"/>
+          <t>Envision Peripherals, Inc</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>OuterInc</t>
+          <t>IntradecoIvory</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Charleston</t>
+          <t>New Jersey</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1766,23 +1912,27 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>OUTER, INC</t>
+          <t>INTRADECO-IVORY</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>OUTER, INC</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr"/>
+          <t>INTRADECO-IVORY</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>ELIXPolymers</t>
+          <t>IntradecoKnothe</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1797,28 +1947,32 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>ELIX POLYMERS AMERICAS LLC</t>
+          <t>INTRADECO-KNOTHE</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>ELIX POLYMERS AMERICAS LLC</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr"/>
+          <t>INTRADECO-KNOTHE</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>ELIXPolymers</t>
+          <t>King'sHawaiian</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>New Jersey</t>
+          <t>Valley View</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1828,59 +1982,65 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>ELIX POLYMERS AMERICAS LLC</t>
+          <t>KING'S HAWAIIAN</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>ELIX POLYMERS AMERICAS LLC</t>
-        </is>
-      </c>
-      <c r="G45" t="inlineStr"/>
+          <t>KING'S HAWAIIAN</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>TheNobleCollection</t>
+          <t>OuterInc</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Fontana</t>
+          <t>Quality 4400</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Bimonthly</t>
+          <t>Weekly</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>THE NOBLE COLLECTION</t>
+          <t>OUTER, INC</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>THE NOBLE COLLECTION</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr"/>
+          <t>OUTER, INC</t>
+        </is>
+      </c>
+      <c r="G46" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>TheNobleCollection</t>
+          <t>Pepsico</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Innovation</t>
+          <t>Tacoma</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1890,108 +2050,674 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>THE NOBLE COLLECTION</t>
+          <t>PEPSICO</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>THE NOBLE COLLECTION</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr"/>
+          <t>PEPSICO</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>NZXT</t>
+          <t>SafeCatch</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Valley View</t>
+          <t>Kent</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Bimonthly</t>
+          <t>Weekly</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>NZXT</t>
+          <t>SAFE CATCH, INC.</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>NZXT</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr"/>
+          <t>SAFE CATCH, INC.</t>
+        </is>
+      </c>
+      <c r="G48" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>E&amp;SInternationalEnterprises</t>
+          <t>SafeCatch</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>New Jersey</t>
+          <t>ViaBaron</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Bimonthly</t>
+          <t>Weekly</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>E&amp;S INTERNATIONAL ENTERPRISES, INC</t>
+          <t>SAFE CATCH, INC.</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>E&amp;S INTERNATIONAL ENTERPRISES, INC (NON-BONDED)</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr"/>
+          <t>SAFE CATCH, INC.</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>SunpowerCorporation</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Innovation</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Weekly</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>SUNPOWER CORPORATION</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>SunPower - Riverside</t>
+        </is>
+      </c>
+      <c r="G50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Surf9LLC</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Lakewood</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Weekly</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>SURF 9 LLC</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>SURF 9 LLC</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>LunaWellnessLLC</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Valley View</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Bimonthly</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Luna Wellness LLC</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Luna Wellness LLC</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>LumistellaCompany</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Morgan Lakes</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Weekly</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>THE LUMISTELLA COMPANY</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>THE LUMISTELLA COMPANY</t>
+        </is>
+      </c>
+      <c r="G53" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>53</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>PassionTree</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Valley View</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Weekly</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>PASSION TREE CO</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>PASSION TREE CO</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>54</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>SharkNinja</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Fontana</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Bimonthly</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Shark Ninja</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>SharkNinja Sales Company</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>OtisMcallister</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Houston</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Bimonthly</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>OTIS MCALLISTER, INC</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>OTIS MCALLISTER, INC</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>OuterInc</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Charleston</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Bimonthly</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>OUTER, INC</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>OUTER, INC</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>57</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>IndianaSugars-NonBonded</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Joilet</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Weekly</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>INDIANA SUGARS- Non Bonded</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>INDIANA SUGARS- Non Bonded</t>
+        </is>
+      </c>
+      <c r="G58" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>58</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>ELIXPolymers</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Morgan Lakes</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Bimonthly</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>ELIX POLYMERS AMERICAS LLC</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>ELIX POLYMERS AMERICAS LLC</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>59</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>ELIXPolymers</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>New Jersey</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Bimonthly</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>ELIX POLYMERS AMERICAS LLC</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>ELIX POLYMERS AMERICAS LLC</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>60</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>TheNobleCollection</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Fontana</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Bimonthly</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>THE NOBLE COLLECTION</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>THE NOBLE COLLECTION</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>TheNobleCollection</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Innovation</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Bimonthly</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>THE NOBLE COLLECTION</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>THE NOBLE COLLECTION</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>RoyalIngredients</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Houston</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Weekly</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>ROYAL INGREDIENTS GROUP USA INC.</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>Royal Ingredients Group USA Inc.</t>
+        </is>
+      </c>
+      <c r="G63" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>63</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>NZXT</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Valley View</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Bimonthly</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>NZXT</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>NZXT</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>64</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>E&amp;SInternationalEnterprises</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>New Jersey</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Bimonthly</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>E&amp;S INTERNATIONAL ENTERPRISES, INC</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>E&amp;S INTERNATIONAL ENTERPRISES, INC (NON-BONDED)</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
         <v>65</v>
       </c>
-      <c r="B50" t="inlineStr">
+      <c r="B66" t="inlineStr">
         <is>
           <t>Turtlebeach</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
+      <c r="C66" t="inlineStr">
         <is>
           <t>Joilet</t>
         </is>
       </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>Bimonthly</t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr">
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Bimonthly</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
         <is>
           <t>TURTLE BEACH</t>
         </is>
       </c>
-      <c r="F50" t="inlineStr">
+      <c r="F66" t="inlineStr">
         <is>
           <t>Turtle Beach</t>
         </is>
       </c>
-      <c r="G50" t="inlineStr"/>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>No BNP Invoice</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>